<commit_message>
modified:   data/ALLQ2024.xlsx modified:   pages/Q1~4_2024_Annual_Report.py
</commit_message>
<xml_diff>
--- a/data/ALLQ2024.xlsx
+++ b/data/ALLQ2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nina/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE0C488-4B6C-CC4F-9534-FEC8FD9C167B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A28CB9-C0AA-314A-8407-7560C6C15E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12100" yWindow="500" windowWidth="16700" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12100" yWindow="560" windowWidth="16700" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="criteria for qualitative assess" sheetId="1" r:id="rId1"/>
@@ -228,14 +228,37 @@
         <r>
           <rPr>
             <sz val="12"/>
-            <color theme="1"/>
+            <color rgb="FF000000"/>
             <rFont val="Aptos Narrow"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>======
-ID#AAABbjCR8sY
-Margarita Sanz    (2025-01-12 13:59:19)
-paper publication: 2022; online publication: October 2024</t>
+          <t xml:space="preserve">======
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Aptos Narrow"/>
+          </rPr>
+          <t xml:space="preserve">ID#AAABbjCR8sY
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Aptos Narrow"/>
+          </rPr>
+          <t xml:space="preserve">Margarita Sanz    (2025-01-12 13:59:19)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Aptos Narrow"/>
+          </rPr>
+          <t>paper publication: 2022; online publication: October 2024</t>
         </r>
       </text>
     </comment>
@@ -244,14 +267,37 @@
         <r>
           <rPr>
             <sz val="12"/>
-            <color theme="1"/>
+            <color rgb="FF000000"/>
             <rFont val="Aptos Narrow"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>======
-ID#AAABbjCR8sc
-Margarita Sanz    (2025-01-12 13:59:19)
-paper publication: 2022; online publication: October 2024</t>
+          <t xml:space="preserve">======
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Aptos Narrow"/>
+          </rPr>
+          <t xml:space="preserve">ID#AAABbjCR8sc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Aptos Narrow"/>
+          </rPr>
+          <t xml:space="preserve">Margarita Sanz    (2025-01-12 13:59:19)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Aptos Narrow"/>
+          </rPr>
+          <t>paper publication: 2022; online publication: October 2024</t>
         </r>
       </text>
     </comment>
@@ -260,14 +306,37 @@
         <r>
           <rPr>
             <sz val="12"/>
-            <color theme="1"/>
+            <color rgb="FF000000"/>
             <rFont val="Aptos Narrow"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>======
-ID#AAABbjCR8sQ
-Margarita Sanz    (2025-01-12 13:59:19)
-paper publication: 2022; online publication: October 2024</t>
+          <t xml:space="preserve">======
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Aptos Narrow"/>
+          </rPr>
+          <t xml:space="preserve">ID#AAABbjCR8sQ
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Aptos Narrow"/>
+          </rPr>
+          <t xml:space="preserve">Margarita Sanz    (2025-01-12 13:59:19)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Aptos Narrow"/>
+          </rPr>
+          <t>paper publication: 2022; online publication: October 2024</t>
         </r>
       </text>
     </comment>
@@ -905,9 +974,6 @@
     <t>posted by 1 X user</t>
   </si>
   <si>
-    <t>31.06.2024</t>
-  </si>
-  <si>
     <t>Conditions of women holding management positions in Poland</t>
   </si>
   <si>
@@ -921,9 +987,6 @@
   </si>
   <si>
     <t>Economic and Regional Studies / Studia Ekonomiczne i Regionalne</t>
-  </si>
-  <si>
-    <t>31.06.2025</t>
   </si>
   <si>
     <t>https://sciendo.com/article/10.2478/ers-2024-0016</t>
@@ -1486,6 +1549,12 @@
   </si>
   <si>
     <t>COLOUR LEGEND</t>
+  </si>
+  <si>
+    <t>30.06.2024</t>
+  </si>
+  <si>
+    <t>30.06.2025</t>
   </si>
 </sst>
 </file>
@@ -2178,7 +2247,7 @@
   <dimension ref="A1:Q978"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2246,7 +2315,7 @@
         <v>15</v>
       </c>
       <c r="Q1" s="32" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3351,22 +3420,22 @@
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="B23" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="C23" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="D23" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="E23" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="F23" s="31" t="s">
         <v>213</v>
-      </c>
-      <c r="F23" s="31" t="s">
-        <v>214</v>
       </c>
       <c r="G23" s="16" t="s">
         <v>33</v>
@@ -3403,22 +3472,22 @@
     </row>
     <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="40" t="s">
-        <v>215</v>
+        <v>388</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C24" s="50" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D24" s="41" t="s">
+        <v>211</v>
+      </c>
+      <c r="E24" s="41" t="s">
         <v>212</v>
       </c>
-      <c r="E24" s="41" t="s">
+      <c r="F24" s="59" t="s">
         <v>213</v>
-      </c>
-      <c r="F24" s="59" t="s">
-        <v>214</v>
       </c>
       <c r="G24" s="41" t="s">
         <v>81</v>
@@ -3455,25 +3524,25 @@
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="C25" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="D25" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="E25" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="F25" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="D25" s="16" t="s">
-        <v>380</v>
-      </c>
-      <c r="E25" s="16" t="s">
+      <c r="G25" s="26" t="s">
         <v>220</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="G25" s="26" t="s">
-        <v>222</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>23</v>
@@ -3493,7 +3562,7 @@
         <v>1</v>
       </c>
       <c r="O25" s="34" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="P25" s="3">
         <f>K27*0.2 + L27*0.4 + M27*0.1 + N27*0.1 + 1*0.2</f>
@@ -3505,25 +3574,25 @@
     </row>
     <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="C26" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="D26" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="E26" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="F26" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="G26" s="16" t="s">
         <v>228</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>230</v>
       </c>
       <c r="H26" s="16" t="s">
         <v>207</v>
@@ -3547,7 +3616,7 @@
         <v>1</v>
       </c>
       <c r="O26" s="34" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="P26" s="3">
         <f>K28*0.2 + L28*0.4 + M28*0.1 + N28*0.1 + 2*0.2</f>
@@ -3559,25 +3628,25 @@
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="C27" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="D27" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="E27" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="F27" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="G27" s="16" t="s">
         <v>236</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>238</v>
       </c>
       <c r="H27" s="16" t="s">
         <v>23</v>
@@ -3613,25 +3682,25 @@
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="46" t="s">
+        <v>230</v>
+      </c>
+      <c r="B28" s="47" t="s">
+        <v>231</v>
+      </c>
+      <c r="C28" s="47" t="s">
         <v>232</v>
       </c>
-      <c r="B28" s="47" t="s">
+      <c r="D28" s="47" t="s">
         <v>233</v>
       </c>
-      <c r="C28" s="47" t="s">
+      <c r="E28" s="47" t="s">
         <v>234</v>
       </c>
-      <c r="D28" s="47" t="s">
+      <c r="F28" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="E28" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="F28" s="47" t="s">
+      <c r="G28" s="47" t="s">
         <v>237</v>
-      </c>
-      <c r="G28" s="47" t="s">
-        <v>239</v>
       </c>
       <c r="H28" s="47" t="s">
         <v>23</v>
@@ -3667,25 +3736,25 @@
     </row>
     <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="C29" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="D29" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="E29" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="F29" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="G29" s="16" t="s">
         <v>244</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>246</v>
       </c>
       <c r="H29" s="16" t="s">
         <v>81</v>
@@ -3721,28 +3790,28 @@
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="C30" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="D30" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="E30" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="F30" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="G30" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="H30" s="16" t="s">
         <v>252</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>253</v>
-      </c>
-      <c r="H30" s="16" t="s">
-        <v>254</v>
       </c>
       <c r="I30" s="3">
         <v>2020</v>
@@ -3773,25 +3842,25 @@
     </row>
     <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C31" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="D31" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="E31" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="F31" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="G31" s="26" t="s">
         <v>259</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="G31" s="26" t="s">
-        <v>261</v>
       </c>
       <c r="H31" s="16" t="s">
         <v>23</v>
@@ -3813,7 +3882,7 @@
         <v>1</v>
       </c>
       <c r="O31" s="34" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="P31" s="3">
         <f>K33*0.2 + L33*0.4 + M33*0.1 + N33*0.1 + 3*0.2</f>
@@ -3825,25 +3894,25 @@
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B32" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="D32" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="E32" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="F32" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="G32" s="26" t="s">
         <v>265</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="G32" s="26" t="s">
-        <v>267</v>
       </c>
       <c r="H32" s="16" t="s">
         <v>23</v>
@@ -3877,28 +3946,28 @@
     </row>
     <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="C33" s="16" t="s">
         <v>268</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="D33" s="16" t="s">
         <v>269</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>270</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>271</v>
       </c>
       <c r="E33" s="16" t="s">
         <v>35</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G33" s="27" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H33" s="27" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="15" t="s">
@@ -3924,25 +3993,25 @@
         <v>45565</v>
       </c>
       <c r="B34" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="D34" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="E34" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="F34" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="E34" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>278</v>
-      </c>
       <c r="G34" s="27" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H34" s="27" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="15" t="s">
@@ -3969,25 +4038,25 @@
         <v>45565</v>
       </c>
       <c r="B35" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="D35" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="E35" s="16" t="s">
         <v>280</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="F35" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="E35" s="16" t="s">
-        <v>282</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>283</v>
-      </c>
       <c r="G35" s="27" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H35" s="27" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="15" t="s">
@@ -4010,25 +4079,25 @@
     </row>
     <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="C36" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="D36" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="E36" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="F36" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="G36" s="16" t="s">
         <v>288</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>289</v>
-      </c>
-      <c r="G36" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="H36" s="16" t="s">
         <v>147</v>
@@ -4064,28 +4133,28 @@
     </row>
     <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="C37" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="D37" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="E37" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="F37" s="16" t="s">
         <v>294</v>
       </c>
-      <c r="E37" s="16" t="s">
+      <c r="G37" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="F37" s="16" t="s">
+      <c r="H37" s="16" t="s">
         <v>296</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="H37" s="16" t="s">
-        <v>298</v>
       </c>
       <c r="I37" s="4">
         <v>2017</v>
@@ -4116,25 +4185,25 @@
     </row>
     <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="C38" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="B38" s="29" t="s">
+      <c r="D38" s="31" t="s">
         <v>300</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="E38" s="31" t="s">
         <v>301</v>
       </c>
-      <c r="D38" s="31" t="s">
+      <c r="F38" s="31" t="s">
         <v>302</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="G38" s="16" t="s">
         <v>303</v>
-      </c>
-      <c r="F38" s="31" t="s">
-        <v>304</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>305</v>
       </c>
       <c r="H38" s="16" t="s">
         <v>148</v>
@@ -4158,7 +4227,7 @@
         <v>1</v>
       </c>
       <c r="O38" s="34" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="P38" s="3">
         <f t="shared" ref="P38:P45" si="4">K38*0.2 + L38*0.4 + M38*0.1 + N38*0.1 + 17* 0.2</f>
@@ -4170,25 +4239,25 @@
     </row>
     <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="B39" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="C39" s="37" t="s">
         <v>299</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="D39" s="53" t="s">
         <v>300</v>
       </c>
-      <c r="C39" s="37" t="s">
+      <c r="E39" s="53" t="s">
         <v>301</v>
       </c>
-      <c r="D39" s="53" t="s">
+      <c r="F39" s="53" t="s">
         <v>302</v>
       </c>
-      <c r="E39" s="53" t="s">
-        <v>303</v>
-      </c>
-      <c r="F39" s="53" t="s">
-        <v>304</v>
-      </c>
       <c r="G39" s="37" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H39" s="37" t="s">
         <v>207</v>
@@ -4212,7 +4281,7 @@
         <v>1</v>
       </c>
       <c r="O39" s="43" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="P39" s="44">
         <f t="shared" si="4"/>
@@ -4224,25 +4293,25 @@
     </row>
     <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="B40" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="C40" s="37" t="s">
         <v>299</v>
       </c>
-      <c r="B40" s="36" t="s">
+      <c r="D40" s="53" t="s">
         <v>300</v>
       </c>
-      <c r="C40" s="37" t="s">
+      <c r="E40" s="53" t="s">
         <v>301</v>
       </c>
-      <c r="D40" s="53" t="s">
+      <c r="F40" s="53" t="s">
         <v>302</v>
       </c>
-      <c r="E40" s="53" t="s">
-        <v>303</v>
-      </c>
-      <c r="F40" s="53" t="s">
-        <v>304</v>
-      </c>
       <c r="G40" s="37" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H40" s="37" t="s">
         <v>148</v>
@@ -4266,7 +4335,7 @@
         <v>1</v>
       </c>
       <c r="O40" s="43" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="P40" s="44">
         <f t="shared" si="4"/>
@@ -4278,25 +4347,25 @@
     </row>
     <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="B41" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="C41" s="37" t="s">
         <v>299</v>
       </c>
-      <c r="B41" s="36" t="s">
+      <c r="D41" s="53" t="s">
         <v>300</v>
       </c>
-      <c r="C41" s="37" t="s">
+      <c r="E41" s="53" t="s">
         <v>301</v>
       </c>
-      <c r="D41" s="53" t="s">
+      <c r="F41" s="53" t="s">
         <v>302</v>
       </c>
-      <c r="E41" s="53" t="s">
-        <v>303</v>
-      </c>
-      <c r="F41" s="53" t="s">
-        <v>304</v>
-      </c>
       <c r="G41" s="37" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H41" s="37" t="s">
         <v>148</v>
@@ -4320,7 +4389,7 @@
         <v>1</v>
       </c>
       <c r="O41" s="43" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="P41" s="44">
         <f t="shared" si="4"/>
@@ -4332,28 +4401,28 @@
     </row>
     <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="B42" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="C42" s="37" t="s">
         <v>299</v>
       </c>
-      <c r="B42" s="36" t="s">
+      <c r="D42" s="53" t="s">
         <v>300</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="E42" s="53" t="s">
         <v>301</v>
       </c>
-      <c r="D42" s="53" t="s">
+      <c r="F42" s="53" t="s">
         <v>302</v>
-      </c>
-      <c r="E42" s="53" t="s">
-        <v>303</v>
-      </c>
-      <c r="F42" s="53" t="s">
-        <v>304</v>
       </c>
       <c r="G42" s="37" t="s">
         <v>33</v>
       </c>
       <c r="H42" s="37" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="I42" s="38" t="s">
         <v>82</v>
@@ -4374,7 +4443,7 @@
         <v>1</v>
       </c>
       <c r="O42" s="43" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="P42" s="44">
         <f t="shared" si="4"/>
@@ -4386,25 +4455,25 @@
     </row>
     <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="B43" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="C43" s="37" t="s">
         <v>299</v>
       </c>
-      <c r="B43" s="36" t="s">
+      <c r="D43" s="53" t="s">
         <v>300</v>
       </c>
-      <c r="C43" s="37" t="s">
+      <c r="E43" s="53" t="s">
         <v>301</v>
       </c>
-      <c r="D43" s="53" t="s">
+      <c r="F43" s="53" t="s">
         <v>302</v>
       </c>
-      <c r="E43" s="53" t="s">
-        <v>303</v>
-      </c>
-      <c r="F43" s="53" t="s">
-        <v>304</v>
-      </c>
       <c r="G43" s="37" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H43" s="37" t="s">
         <v>81</v>
@@ -4428,7 +4497,7 @@
         <v>1</v>
       </c>
       <c r="O43" s="43" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="P43" s="44">
         <f t="shared" si="4"/>
@@ -4440,25 +4509,25 @@
     </row>
     <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="B44" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="C44" s="37" t="s">
         <v>299</v>
       </c>
-      <c r="B44" s="36" t="s">
+      <c r="D44" s="53" t="s">
         <v>300</v>
       </c>
-      <c r="C44" s="37" t="s">
+      <c r="E44" s="53" t="s">
         <v>301</v>
       </c>
-      <c r="D44" s="53" t="s">
+      <c r="F44" s="53" t="s">
         <v>302</v>
       </c>
-      <c r="E44" s="53" t="s">
-        <v>303</v>
-      </c>
-      <c r="F44" s="53" t="s">
-        <v>304</v>
-      </c>
       <c r="G44" s="37" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H44" s="37" t="s">
         <v>207</v>
@@ -4482,7 +4551,7 @@
         <v>1</v>
       </c>
       <c r="O44" s="43" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="P44" s="44">
         <f t="shared" si="4"/>
@@ -4494,25 +4563,25 @@
     </row>
     <row r="45" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="B45" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="C45" s="37" t="s">
         <v>299</v>
       </c>
-      <c r="B45" s="36" t="s">
+      <c r="D45" s="53" t="s">
         <v>300</v>
       </c>
-      <c r="C45" s="37" t="s">
+      <c r="E45" s="53" t="s">
         <v>301</v>
       </c>
-      <c r="D45" s="53" t="s">
+      <c r="F45" s="53" t="s">
         <v>302</v>
       </c>
-      <c r="E45" s="53" t="s">
-        <v>303</v>
-      </c>
-      <c r="F45" s="53" t="s">
-        <v>304</v>
-      </c>
       <c r="G45" s="37" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="H45" s="37" t="s">
         <v>23</v>
@@ -4536,7 +4605,7 @@
         <v>1</v>
       </c>
       <c r="O45" s="43" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="P45" s="44">
         <f t="shared" si="4"/>
@@ -4548,25 +4617,25 @@
     </row>
     <row r="46" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>312</v>
+      </c>
+      <c r="C46" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="D46" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="E46" s="16" t="s">
         <v>314</v>
       </c>
-      <c r="C46" s="16" t="s">
+      <c r="F46" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="D46" s="16" t="s">
-        <v>381</v>
-      </c>
-      <c r="E46" s="16" t="s">
+      <c r="G46" s="16" t="s">
         <v>316</v>
-      </c>
-      <c r="F46" s="16" t="s">
-        <v>317</v>
-      </c>
-      <c r="G46" s="16" t="s">
-        <v>318</v>
       </c>
       <c r="H46" s="16" t="s">
         <v>23</v>
@@ -4600,28 +4669,28 @@
     </row>
     <row r="47" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="C47" s="16" t="s">
         <v>319</v>
       </c>
-      <c r="B47" s="16" t="s">
+      <c r="D47" s="16" t="s">
         <v>320</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="E47" s="16" t="s">
         <v>321</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="F47" s="16" t="s">
         <v>322</v>
       </c>
-      <c r="E47" s="16" t="s">
-        <v>323</v>
-      </c>
-      <c r="F47" s="16" t="s">
-        <v>324</v>
-      </c>
       <c r="G47" s="27" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H47" s="27" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I47" s="4"/>
       <c r="J47" s="18" t="s">
@@ -4646,28 +4715,28 @@
     </row>
     <row r="48" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="C48" s="16" t="s">
         <v>325</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="D48" s="16" t="s">
+        <v>380</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="F48" s="16" t="s">
         <v>326</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="G48" s="16" t="s">
         <v>327</v>
       </c>
-      <c r="D48" s="16" t="s">
-        <v>382</v>
-      </c>
-      <c r="E48" s="16" t="s">
-        <v>384</v>
-      </c>
-      <c r="F48" s="16" t="s">
+      <c r="H48" s="16" t="s">
         <v>328</v>
-      </c>
-      <c r="G48" s="16" t="s">
-        <v>329</v>
-      </c>
-      <c r="H48" s="16" t="s">
-        <v>330</v>
       </c>
       <c r="I48" s="4">
         <v>2018</v>
@@ -4692,25 +4761,25 @@
     </row>
     <row r="49" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>330</v>
+      </c>
+      <c r="C49" s="16" t="s">
         <v>331</v>
       </c>
-      <c r="B49" s="16" t="s">
+      <c r="D49" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="E49" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="D49" s="16" t="s">
+      <c r="F49" s="16" t="s">
         <v>334</v>
       </c>
-      <c r="E49" s="16" t="s">
+      <c r="G49" s="25" t="s">
         <v>335</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>336</v>
-      </c>
-      <c r="G49" s="25" t="s">
-        <v>337</v>
       </c>
       <c r="H49" s="16" t="s">
         <v>23</v>
@@ -4732,7 +4801,7 @@
       </c>
       <c r="N49" s="34"/>
       <c r="O49" s="34" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="P49" s="3">
         <f>K49*0.2 + L49*0.4 + M49*0.1 + N49*0.1 + 5 *0.2</f>
@@ -4744,28 +4813,28 @@
     </row>
     <row r="50" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="C50" s="16" t="s">
         <v>339</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="D50" s="16" t="s">
         <v>340</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="E50" s="16" t="s">
         <v>341</v>
       </c>
-      <c r="D50" s="16" t="s">
+      <c r="F50" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="G50" s="25" t="s">
         <v>342</v>
       </c>
-      <c r="E50" s="16" t="s">
+      <c r="H50" s="16" t="s">
         <v>343</v>
-      </c>
-      <c r="F50" s="16" t="s">
-        <v>328</v>
-      </c>
-      <c r="G50" s="25" t="s">
-        <v>344</v>
-      </c>
-      <c r="H50" s="16" t="s">
-        <v>345</v>
       </c>
       <c r="I50" s="4">
         <v>2017</v>
@@ -4784,7 +4853,7 @@
         <v>1</v>
       </c>
       <c r="O50" s="34" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="P50" s="3">
         <f t="shared" ref="P50:P51" si="6">K50*0.2 + L50*0.4 + M50*0.1 + N50*0.1 + 11*0.2</f>
@@ -4796,28 +4865,28 @@
     </row>
     <row r="51" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="40" t="s">
+        <v>337</v>
+      </c>
+      <c r="B51" s="36" t="s">
+        <v>338</v>
+      </c>
+      <c r="C51" s="41" t="s">
         <v>339</v>
       </c>
-      <c r="B51" s="36" t="s">
+      <c r="D51" s="41" t="s">
         <v>340</v>
       </c>
-      <c r="C51" s="41" t="s">
+      <c r="E51" s="55" t="s">
         <v>341</v>
       </c>
-      <c r="D51" s="41" t="s">
-        <v>342</v>
-      </c>
-      <c r="E51" s="55" t="s">
-        <v>343</v>
-      </c>
       <c r="F51" s="41" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G51" s="37" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="H51" s="41" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="I51" s="42">
         <v>2023</v>
@@ -4836,7 +4905,7 @@
         <v>1</v>
       </c>
       <c r="O51" s="58" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="P51" s="44">
         <f t="shared" si="6"/>
@@ -4848,28 +4917,28 @@
     </row>
     <row r="52" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="C52" s="16" t="s">
         <v>349</v>
       </c>
-      <c r="B52" s="16" t="s">
+      <c r="D52" s="16" t="s">
         <v>350</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="E52" s="16" t="s">
         <v>351</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="F52" s="16" t="s">
         <v>352</v>
       </c>
-      <c r="E52" s="16" t="s">
-        <v>353</v>
-      </c>
-      <c r="F52" s="16" t="s">
-        <v>354</v>
-      </c>
       <c r="G52" s="27" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H52" s="27" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I52" s="4"/>
       <c r="J52" s="18" t="s">
@@ -4892,28 +4961,28 @@
     </row>
     <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="C53" s="16" t="s">
         <v>355</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="D53" s="16" t="s">
         <v>356</v>
       </c>
-      <c r="C53" s="16" t="s">
+      <c r="E53" s="16" t="s">
         <v>357</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="F53" s="16" t="s">
         <v>358</v>
       </c>
-      <c r="E53" s="16" t="s">
-        <v>359</v>
-      </c>
-      <c r="F53" s="16" t="s">
-        <v>360</v>
-      </c>
       <c r="G53" s="27" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H53" s="27" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I53" s="4"/>
       <c r="J53" s="18" t="s">
@@ -4931,30 +5000,30 @@
         <v>0</v>
       </c>
       <c r="Q53" s="4" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="54" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="C54" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="D54" s="16" t="s">
         <v>363</v>
       </c>
-      <c r="C54" s="16" t="s">
+      <c r="E54" s="16" t="s">
         <v>364</v>
       </c>
-      <c r="D54" s="16" t="s">
+      <c r="F54" s="16" t="s">
         <v>365</v>
       </c>
-      <c r="E54" s="16" t="s">
+      <c r="G54" s="16" t="s">
         <v>366</v>
-      </c>
-      <c r="F54" s="16" t="s">
-        <v>367</v>
-      </c>
-      <c r="G54" s="16" t="s">
-        <v>368</v>
       </c>
       <c r="H54" s="16" t="s">
         <v>66</v>
@@ -4990,25 +5059,25 @@
     </row>
     <row r="55" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B55" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="D55" s="16" t="s">
         <v>369</v>
       </c>
-      <c r="C55" s="16" t="s">
+      <c r="E55" s="16" t="s">
         <v>370</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="F55" s="16" t="s">
         <v>371</v>
       </c>
-      <c r="E55" s="16" t="s">
-        <v>372</v>
-      </c>
-      <c r="F55" s="16" t="s">
-        <v>373</v>
-      </c>
       <c r="G55" s="16" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H55" s="16" t="s">
         <v>23</v>
@@ -5042,28 +5111,28 @@
     </row>
     <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B56" s="16" t="s">
+        <v>372</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>373</v>
+      </c>
+      <c r="D56" s="16" t="s">
         <v>374</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="E56" s="16" t="s">
         <v>375</v>
       </c>
-      <c r="D56" s="16" t="s">
+      <c r="F56" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="E56" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="F56" s="16" t="s">
-        <v>378</v>
-      </c>
       <c r="G56" s="27" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H56" s="27" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I56" s="4"/>
       <c r="J56" s="18" t="s">
@@ -5074,7 +5143,7 @@
       <c r="M56" s="62"/>
       <c r="N56" s="63"/>
       <c r="O56" s="34" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="P56" s="3">
         <f>K56*0.2 + L56*0.4 + M56*0.1 + N56*0.1 + 22*0.2</f>
@@ -5124,7 +5193,7 @@
     </row>
     <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="75" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B59" s="76"/>
       <c r="C59" s="16"/>
@@ -5146,7 +5215,7 @@
     <row r="60" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="70"/>
       <c r="B60" s="71" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C60" s="16"/>
       <c r="D60" s="16"/>
@@ -5167,7 +5236,7 @@
     <row r="61" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="72"/>
       <c r="B61" s="71" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C61" s="16"/>
       <c r="D61" s="16"/>
@@ -5188,7 +5257,7 @@
     <row r="62" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="73"/>
       <c r="B62" s="74" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C62" s="16"/>
       <c r="D62" s="16"/>

</xml_diff>